<commit_message>
Added internal deadlines to release plan
</commit_message>
<xml_diff>
--- a/doc/ReleasePlan.xlsx
+++ b/doc/ReleasePlan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spack\Documents\CMPUT301\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Lafrance\Documents\School\Computer Science 301\PraiseTheSun\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10296" windowHeight="2664" xr2:uid="{306B7C16-71B4-4FE4-ACCC-20A13BB53280}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10300" windowHeight="2660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>Project Part</t>
   </si>
@@ -65,15 +65,9 @@
     <t>US 01.02.01</t>
   </si>
   <si>
-    <t>17: Search for Avilable Tasks</t>
-  </si>
-  <si>
     <t>1: Authenticate</t>
   </si>
   <si>
-    <t>4: View User Conatct Info</t>
-  </si>
-  <si>
     <t>2: Create Account</t>
   </si>
   <si>
@@ -183,13 +177,43 @@
   </si>
   <si>
     <t>US 10.02.01</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>17: Search for Available Tasks</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>4: View User Contact Info</t>
+  </si>
+  <si>
+    <t>Week 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +229,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +251,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -310,16 +348,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -342,6 +434,49 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,269 +791,325 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05541085-EC6A-42EF-A1B0-BB17625022FD}">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C1" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="15"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="16"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="16"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="16"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="17"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="16"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="16"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5" t="s">
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="16"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="16"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="18"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="18"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="18"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="18"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="5" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="18"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="18"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="D26" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="D27" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="18"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5" t="s">
+      <c r="D28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="18"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="18"/>
+      <c r="C30" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>52</v>
-      </c>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made a few changes to the ReleasePlan.xlsx
</commit_message>
<xml_diff>
--- a/doc/ReleasePlan.xlsx
+++ b/doc/ReleasePlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Project Part</t>
   </si>
@@ -134,12 +134,6 @@
     <t>Project Part 5</t>
   </si>
   <si>
-    <t>25: Set Task Status to Done</t>
-  </si>
-  <si>
-    <t>26: Set Task Status to Requested</t>
-  </si>
-  <si>
     <t>US 07.01.01</t>
   </si>
   <si>
@@ -207,6 +201,15 @@
   </si>
   <si>
     <t>Week 6</t>
+  </si>
+  <si>
+    <t>25: Change status for one of my tasks</t>
+  </si>
+  <si>
+    <t>26: Wow factor</t>
+  </si>
+  <si>
+    <t>US Wow Factor</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,14 +254,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -405,11 +402,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -475,7 +481,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,12 +820,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C1" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -833,7 +845,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -889,7 +901,7 @@
       <c r="A9" s="16"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
@@ -897,7 +909,7 @@
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="4" t="s">
@@ -931,7 +943,7 @@
       <c r="A13" s="16"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>18</v>
@@ -939,7 +951,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="4" t="s">
@@ -987,54 +999,58 @@
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="18"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>30</v>
+      <c r="C22" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" s="14"/>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1044,72 +1060,62 @@
         <v>37</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="18"/>
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="18"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D26" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="18"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
       <c r="B28" s="1"/>
       <c r="C28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
-      <c r="B29" s="1"/>
       <c r="C29" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
-      <c r="C30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C33" s="10"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C32" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edited release plan and updated photo
</commit_message>
<xml_diff>
--- a/doc/ReleasePlan.xlsx
+++ b/doc/ReleasePlan.xlsx
@@ -255,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -347,26 +347,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -378,6 +358,104 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -388,22 +466,33 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -415,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -441,15 +530,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,37 +542,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,318 +907,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="9" t="s">
+    <row r="2" spans="2:5" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="22"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="24"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="16"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="25"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="25"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="25"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="16"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
+    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="25"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="11" t="s">
+    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="16"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="25"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="4" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="27"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="16"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="4" t="s">
+    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="25"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11" t="s">
+    <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="4" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="25"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="16"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="4" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="25"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="4" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="25"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="18"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="4" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="29"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="18"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="29"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="18"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="25" t="s">
+    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="29"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="E23" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="11" t="s">
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="23" t="s">
+      <c r="C24" s="12"/>
+      <c r="D24" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="18"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="29"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="18"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="29"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="11" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="32"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="29"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="18"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="18"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="12"/>
+      <c r="D29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
-      <c r="C29" s="4" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C32" s="10"/>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small change to release plan
</commit_message>
<xml_diff>
--- a/doc/ReleasePlan.xlsx
+++ b/doc/ReleasePlan.xlsx
@@ -134,9 +134,6 @@
     <t>Project Part 5</t>
   </si>
   <si>
-    <t>US 07.01.01</t>
-  </si>
-  <si>
     <t>23: View Task Assigned</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>US Wow Factor</t>
+  </si>
+  <si>
+    <t>US 07.01.01, US 07.02.01</t>
   </si>
 </sst>
 </file>
@@ -910,7 +910,7 @@
   <dimension ref="B2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,13 +925,13 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="19"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -1007,7 +1007,7 @@
       <c r="B10" s="25"/>
       <c r="C10" s="1"/>
       <c r="D10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>20</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="4" t="s">
@@ -1049,7 +1049,7 @@
       <c r="B14" s="25"/>
       <c r="C14" s="1"/>
       <c r="D14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>18</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="4" t="s">
@@ -1105,7 +1105,7 @@
     </row>
     <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>35</v>
@@ -1141,84 +1141,84 @@
       <c r="B23" s="29"/>
       <c r="C23" s="1"/>
       <c r="D23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="29"/>
       <c r="C25" s="1"/>
       <c r="D25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="29"/>
       <c r="C26" s="1"/>
       <c r="D26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="32"/>
       <c r="C27" s="33"/>
       <c r="D27" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="29"/>
       <c r="C28" s="1"/>
       <c r="D28" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="30"/>
       <c r="C30" s="31"/>
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added project part 2 and 3 to ReleasePlan. Created JavaDoc for TaskList
</commit_message>
<xml_diff>
--- a/doc/ReleasePlan.xlsx
+++ b/doc/ReleasePlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Project Part</t>
   </si>
@@ -32,12 +32,6 @@
     <t>Project Part 4</t>
   </si>
   <si>
-    <t>Use Case</t>
-  </si>
-  <si>
-    <t>Related Artifacts</t>
-  </si>
-  <si>
     <t>US 01.01.01, US 02.02.01, US 08.01.01</t>
   </si>
   <si>
@@ -210,6 +204,45 @@
   </si>
   <si>
     <t>US 07.01.01, US 07.02.01</t>
+  </si>
+  <si>
+    <t>Related Artifacts (if any)</t>
+  </si>
+  <si>
+    <t>Use Case or Description</t>
+  </si>
+  <si>
+    <t>Project Part 2</t>
+  </si>
+  <si>
+    <t>Finish Use Cases</t>
+  </si>
+  <si>
+    <t>Finish User Interface Mockup and Storyboard</t>
+  </si>
+  <si>
+    <t>Finish Release Plan</t>
+  </si>
+  <si>
+    <t>Finish Glossary</t>
+  </si>
+  <si>
+    <t>Project Part 3</t>
+  </si>
+  <si>
+    <t>Respond to feedback</t>
+  </si>
+  <si>
+    <t>Finish UML</t>
+  </si>
+  <si>
+    <t>Create test cases for entity classes</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
   </si>
 </sst>
 </file>
@@ -241,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -490,13 +529,110 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -504,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -512,9 +648,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -532,9 +665,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -570,12 +700,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -591,8 +715,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E33"/>
+  <dimension ref="B2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -922,307 +1108,383 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="19"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="21" t="s">
-        <v>49</v>
+      <c r="B3" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="20"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="2:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="40"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" spans="2:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="49"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="29"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="23"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="21"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="21"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="22"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
+    <row r="19" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="21"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="24"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="21"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="25"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="25"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="E21" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="21"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="23"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="21"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="25"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="25"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="E25" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="21"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="4" t="s">
+      <c r="E26" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="21"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="21"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="25"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="25"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="25"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="25"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="25"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="25"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="26"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="25"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="27"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4" t="s">
+      <c r="E39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="25"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="25"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="25"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="25"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="29"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="29"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="29"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" s="29"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="29"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D33" s="9"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D41" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made a few small changes to ReleasePlan.xlsx
</commit_message>
<xml_diff>
--- a/doc/ReleasePlan.xlsx
+++ b/doc/ReleasePlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Project Part</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Week 8</t>
+  </si>
+  <si>
+    <t>Testing and revisions based on feedback</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -634,6 +637,32 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -654,9 +683,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -669,9 +695,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -679,9 +702,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,8 +733,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -777,6 +795,17 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1093,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E41"/>
+  <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1108,117 +1137,117 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="17"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="20"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="2:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="34" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="2:5" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="32"/>
-    </row>
-    <row r="6" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="40"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="35"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="32"/>
-    </row>
-    <row r="7" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="37"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="33" t="s">
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="32"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="37"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="33" t="s">
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="32"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="2:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
-    </row>
-    <row r="10" spans="2:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="34" t="s">
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="2:5" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="2:5" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="32"/>
-    </row>
-    <row r="11" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="33" t="s">
+      <c r="E10" s="27"/>
+    </row>
+    <row r="11" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="32"/>
-    </row>
-    <row r="12" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="33" t="s">
+      <c r="E11" s="27"/>
+    </row>
+    <row r="12" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="32"/>
-    </row>
-    <row r="13" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="49"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="44"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1226,8 +1255,8 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="29"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1236,8 +1265,8 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="23"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="3" t="s">
         <v>51</v>
       </c>
@@ -1246,7 +1275,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="21"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3" t="s">
         <v>5</v>
@@ -1256,7 +1285,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="21"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3" t="s">
         <v>6</v>
@@ -1266,7 +1295,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="21"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3" t="s">
         <v>9</v>
@@ -1276,215 +1305,255 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="20"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="21"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="21"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="1"/>
       <c r="D22" s="3" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="23"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="1"/>
       <c r="D23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="21"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="20"/>
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="18"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="22" t="s">
+    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="3" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="20"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" s="21"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="21"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" s="21"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="1"/>
       <c r="D28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="18"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="18"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="24" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="22"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" s="25"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="3" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="22"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" s="25"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="25"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="25"/>
+      <c r="B35" s="22"/>
       <c r="C35" s="1"/>
       <c r="D35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="22"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="48"/>
+      <c r="D37" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="20"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="22"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="25"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="3" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="22"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="25"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="3" t="s">
+    <row r="41" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="22"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="22" t="s">
+    <row r="42" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="3" t="s">
+      <c r="C42" s="48"/>
+      <c r="D42" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="20"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="3" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="46"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D41" s="8"/>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D46" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>